<commit_message>
updatd mult compe ahab for lmb
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/habitat/lmb/glmm_multi_comp_hab_LMB.xlsx
+++ b/results/accel-glmm-results/habitat/lmb/glmm_multi_comp_hab_LMB.xlsx
@@ -1,85 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\CU\Data\toronto-lmb-np-accel\results\accel-glmm-results\habitat\lmb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1C2AE6-9637-4E56-BA6B-CAD6D183C106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t xml:space="preserve">term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contrast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">std_error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">df</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">statistic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adj_p_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">habitat_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Mod/Dense SAV) / (Shallow/Low SAV)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Deep/Low SAV) / (Mod/Dense SAV)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Exposed/Low SAV) / (Shallow/Low SAV)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Deep/Low SAV) / (Exposed/Low SAV)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Mod/Dense SAV) / (Shallow/Dense SAV)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Deep/Low SAV) / (Shallow/Low SAV)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Exposed/Low SAV) / (Shallow/Dense SAV)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Shallow/Dense SAV) / (Shallow/Low SAV)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Deep/Low SAV) / (Shallow/Dense SAV)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Exposed/Low SAV) / (Mod/Dense SAV)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>contrast</t>
+  </si>
+  <si>
+    <t>null_value</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>std_error</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>statistic</t>
+  </si>
+  <si>
+    <t>adj_p_value</t>
+  </si>
+  <si>
+    <t>habitat_type</t>
+  </si>
+  <si>
+    <t>(Mod/Dense SAV) / (Shallow/Low SAV)</t>
+  </si>
+  <si>
+    <t>(Deep/Low SAV) / (Mod/Dense SAV)</t>
+  </si>
+  <si>
+    <t>(Exposed/Low SAV) / (Shallow/Low SAV)</t>
+  </si>
+  <si>
+    <t>(Deep/Low SAV) / (Exposed/Low SAV)</t>
+  </si>
+  <si>
+    <t>(Mod/Dense SAV) / (Shallow/Dense SAV)</t>
+  </si>
+  <si>
+    <t>(Deep/Low SAV) / (Shallow/Low SAV)</t>
+  </si>
+  <si>
+    <t>(Exposed/Low SAV) / (Shallow/Dense SAV)</t>
+  </si>
+  <si>
+    <t>(Shallow/Dense SAV) / (Shallow/Low SAV)</t>
+  </si>
+  <si>
+    <t>(Deep/Low SAV) / (Shallow/Dense SAV)</t>
+  </si>
+  <si>
+    <t>(Exposed/Low SAV) / (Mod/Dense SAV)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -115,6 +135,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,14 +425,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,298 +466,298 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>1.68503887583207</v>
       </c>
-      <c r="E2" t="n">
-        <v>0.086147187808556</v>
+      <c r="E2">
+        <v>8.6147187808556E-2</v>
       </c>
       <c r="F2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>10.2061849925406</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.0000000000000000000000186036193505387</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>10.206184992540599</v>
+      </c>
+      <c r="I2">
+        <v>1.86036193505387E-23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.624630754096402</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.0319909114252437</v>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.62463075409640201</v>
+      </c>
+      <c r="E3">
+        <v>3.1990911425243698E-2</v>
       </c>
       <c r="F3" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>-9.18848026130133</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.000000000000000000398430386407911</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>-9.1884802613013292</v>
+      </c>
+      <c r="I3">
+        <v>3.98430386407911E-19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>1.58501640428156</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.082418995368956</v>
+      <c r="E4">
+        <v>8.2418995368956E-2</v>
       </c>
       <c r="F4" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>8.85779112292578</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.00000000000000000816154579527604</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>8.8577911229257804</v>
+      </c>
+      <c r="I4">
+        <v>8.1615457952760396E-18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.664048082309799</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.0345732373820015</v>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.66404808230979895</v>
+      </c>
+      <c r="E5">
+        <v>3.45732373820015E-2</v>
       </c>
       <c r="F5" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>-7.86335856695131</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.0000000000000373968542593598</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>-7.8633585669513097</v>
+      </c>
+      <c r="I5">
+        <v>3.7396854259359797E-14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1.46332923638528</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.0783665725449887</v>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1.4633292363852799</v>
+      </c>
+      <c r="E6">
+        <v>7.8366572544988702E-2</v>
       </c>
       <c r="F6" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>7.10902763437087</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.000000000011686334901397</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>7.1090276343708698</v>
+      </c>
+      <c r="I6">
+        <v>1.1686334901396999E-11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1.05252710369274</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.00927429940320084</v>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1.0525271036927399</v>
+      </c>
+      <c r="E7">
+        <v>9.2742994032008405E-3</v>
       </c>
       <c r="F7" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>5.80993886095569</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.0000000624956612293004</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>5.8099388609556897</v>
+      </c>
+      <c r="I7">
+        <v>6.2495661229300402E-8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.37646726007443</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.0848150388225556</v>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1.3764672600744301</v>
+      </c>
+      <c r="E8">
+        <v>8.4815038822555602E-2</v>
       </c>
       <c r="F8" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>5.18550935648084</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.00000215425271072183</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>5.1855093564808401</v>
+      </c>
+      <c r="I8">
+        <v>2.1542527107218301E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1.15151042836707</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.0557122049755158</v>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1.1515104283670701</v>
+      </c>
+      <c r="E9">
+        <v>5.5712204975515801E-2</v>
       </c>
       <c r="F9" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="n">
-        <v>2.9158557635385</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.0354714443258536</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>2.9158557635385001</v>
+      </c>
+      <c r="I9">
+        <v>3.5471444325853599E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.914040444414649</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.0442523314667095</v>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0.91404044441464904</v>
+      </c>
+      <c r="E10">
+        <v>4.4252331466709503E-2</v>
       </c>
       <c r="F10" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" t="n">
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>-1.85649821377378</v>
       </c>
-      <c r="I10" t="n">
-        <v>0.633825773890801</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="I10">
+        <v>0.63382577389080097</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.940640852276407</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.0628554162725546</v>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.94064085227640704</v>
+      </c>
+      <c r="E11">
+        <v>6.2855416272554601E-2</v>
       </c>
       <c r="F11" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" t="n">
-        <v>-0.915775683657076</v>
-      </c>
-      <c r="I11" t="n">
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>-0.91577568365707596</v>
+      </c>
+      <c r="I11">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>